<commit_message>
Update SMM prices all
</commit_message>
<xml_diff>
--- a/example notebooks/Example publication - integrated modelling/data/ODYM_database/3_PR_material_price_mass_v1.xlsx
+++ b/example notebooks/Example publication - integrated modelling/data/ODYM_database/3_PR_material_price_mass_v1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{91C67D38-4125-4596-B453-F84DCFB4E8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05676D1E-4D6F-492D-9F8F-5FFCF35D7BE8}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="13_ncr:1_{91C67D38-4125-4596-B453-F84DCFB4E8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DADC458-4124-4A52-8F54-12D2CF5BA3A3}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet2!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Values_Master!$A$1:$E$1</definedName>
     <definedName name="_rho_Al">[1]Lists!$H$21</definedName>
     <definedName name="_rho_Cu">[1]Lists!$H$22</definedName>
   </definedNames>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="246">
   <si>
     <t>Date created</t>
   </si>
@@ -644,21 +645,9 @@
     <t>price (kg)</t>
   </si>
   <si>
-    <t>SMM, 3-1-22</t>
-  </si>
-  <si>
     <t>Calculated, see appendix</t>
   </si>
   <si>
-    <t>SMM, 3-1-22  high-end graphite</t>
-  </si>
-  <si>
-    <t>SMM, 3-1-22,  calculated 50% NMC532-50%LMO</t>
-  </si>
-  <si>
-    <t>SMM, 3-1-22 (capacity grade for BEV)</t>
-  </si>
-  <si>
     <t>cathode current collector Al (10um)</t>
   </si>
   <si>
@@ -677,15 +666,6 @@
     <t>cathode current collector Al (18um)</t>
   </si>
   <si>
-    <t>SMM, 3-1-22, based on 12 um Al foil for LIB</t>
-  </si>
-  <si>
-    <t>SMM, 3-1-22, based on 13 um Al foil for LIB</t>
-  </si>
-  <si>
-    <t>SMM, 3-1-22, based on 15 um Al foil for LIB</t>
-  </si>
-  <si>
     <t>anode current collector Cu (10um)</t>
   </si>
   <si>
@@ -707,12 +687,6 @@
     <t>anode current collector Cu (9um)</t>
   </si>
   <si>
-    <t>SMM, 3-1-22, based on a treatment charge for 6 um Cu foil (LIB) and 9.72 $/kg for LME Cu</t>
-  </si>
-  <si>
-    <t>SMM, 3-1-22, based on a treatment charge for 8 um Cu foil (LIB) and 9.72 $/kg for LME Cu</t>
-  </si>
-  <si>
     <t>BatPaC value seems based on old, higher prices. Here  Alibaba price for TYT-3 carbon black min order 16 t. Similar to Greenwood</t>
   </si>
   <si>
@@ -737,9 +711,6 @@
     <t>cooling panels</t>
   </si>
   <si>
-    <t>cooling mains fe</t>
-  </si>
-  <si>
     <t>cooling connectors</t>
   </si>
   <si>
@@ -780,6 +751,102 @@
   </si>
   <si>
     <t>cooling mains Fe</t>
+  </si>
+  <si>
+    <t>SMM 13/05/2022</t>
+  </si>
+  <si>
+    <t>SMM 13/05/2022, high-end graphite</t>
+  </si>
+  <si>
+    <t>SMM 13/05/2022, capacity grade</t>
+  </si>
+  <si>
+    <t>SMM, 13/05/2022,  calculated 50% NMC532-50%LMO</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SMM, 13/05/2022, based on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> um Al foil for LIB and 2.7 $/kg for LME Al</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SMM, 13/05/2022, based on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> um Al foil for LIB and 2.7 $/kg for LME Al</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SMM, 13/05/2022, based on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> um Al foil for LIB and 2.7 $/kg for LME Al</t>
+    </r>
+  </si>
+  <si>
+    <t>SMM, 13/05/2022, based on a treatment charge for 6 um Cu foil (LIB) and 9.00 $/kg for LME Cu</t>
+  </si>
+  <si>
+    <t>SMM, 13/05/2022, based on a treatment charge for 8 um Cu foil (LIB) and 9.00 $/kg for LME Cu</t>
   </si>
 </sst>
 </file>
@@ -797,7 +864,7 @@
     <numFmt numFmtId="170" formatCode="0.000"/>
     <numFmt numFmtId="171" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -933,6 +1000,12 @@
       <color rgb="FFA31515"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF303133"/>
+      <name val="Lato"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1082,7 +1155,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1145,6 +1218,18 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="36">
     <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2043,8 +2128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BDDE9FA-34B5-487F-BD06-B5E05371CD58}">
   <dimension ref="A1:O87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A1:E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2092,784 +2177,789 @@
         <v>139</v>
       </c>
       <c r="B2" s="39">
-        <v>9.1001999999999992</v>
+        <v>9.1166199999999993</v>
       </c>
       <c r="C2" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="35" t="s">
-        <v>203</v>
+      <c r="D2" s="53" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B3" s="39">
-        <v>12.15972</v>
+        <v>60</v>
       </c>
       <c r="C3" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>203</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4" s="39">
-        <v>60</v>
+        <v>12.15058</v>
       </c>
       <c r="C4" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="D4" t="s">
-        <v>162</v>
+      <c r="D4" s="53" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B5" s="39">
-        <v>10.98298</v>
+        <v>5</v>
       </c>
       <c r="C5" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>205</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="B6" s="39">
-        <v>15.532999999999999</v>
+        <v>5</v>
       </c>
       <c r="C6" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>201</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:15" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
-        <v>144</v>
-      </c>
-      <c r="B7" s="35">
-        <v>39.64</v>
-      </c>
-      <c r="C7" s="35" t="s">
+      <c r="A7" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="39">
+        <v>3.6</v>
+      </c>
+      <c r="C7" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>202</v>
+        <v>216</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
-        <v>145</v>
+        <v>208</v>
       </c>
       <c r="B8" s="39">
-        <v>42.31</v>
+        <v>14.15479</v>
       </c>
       <c r="C8" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D8" t="s">
-        <v>202</v>
-      </c>
-      <c r="E8" s="35"/>
+        <v>245</v>
+      </c>
+      <c r="E8" s="39"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
-        <v>146</v>
+        <v>209</v>
       </c>
       <c r="B9" s="39">
-        <v>37.969720000000002</v>
+        <v>14.15479</v>
       </c>
       <c r="C9" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D9" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="E9" s="39"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="B10" s="54">
+        <v>14.15479</v>
+      </c>
+      <c r="C10" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="E10" s="39"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="B11" s="54">
+        <v>14.15479</v>
+      </c>
+      <c r="C11" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="E11" s="39"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="B12" s="54">
+        <v>14.15479</v>
+      </c>
+      <c r="C12" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="E12" s="39"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" s="56">
+        <v>15.77487</v>
+      </c>
+      <c r="C13" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="E13" s="39"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="B14" s="56">
+        <v>15.77487</v>
+      </c>
+      <c r="C14" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="E14" s="39"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" s="54">
+        <v>14.15479</v>
+      </c>
+      <c r="C15" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="E15" s="39"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="B16" s="54">
+        <v>14.15479</v>
+      </c>
+      <c r="C16" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="E16" s="39"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="B17" s="12">
+        <v>2.81</v>
+      </c>
+      <c r="C17" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="E17" s="35"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B18" s="12">
+        <v>1.4</v>
+      </c>
+      <c r="C18" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="E18" s="35"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="B19" s="12">
+        <v>9.375</v>
+      </c>
+      <c r="C19" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="57" t="s">
+        <v>165</v>
+      </c>
+      <c r="B20" s="54">
+        <v>0</v>
+      </c>
+      <c r="C20" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="E20" s="35"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="B21" s="54">
+        <v>2.7</v>
+      </c>
+      <c r="C21" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="E21" s="35"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="B22" s="54">
+        <v>8.68</v>
+      </c>
+      <c r="C22" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="E22" s="35"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="B23" s="54">
+        <v>34.021619999999999</v>
+      </c>
+      <c r="C23" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="E23" s="35"/>
+    </row>
+    <row r="24" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B24" s="54">
+        <v>21.429200000000002</v>
+      </c>
+      <c r="C24" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="58" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" s="54">
+        <v>16.642610000000001</v>
+      </c>
+      <c r="C25" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="58" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" s="54">
+        <v>62.7</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="E9" s="35"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
+    </row>
+    <row r="27" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B27" s="54">
+        <v>54.34</v>
+      </c>
+      <c r="C27" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B28" s="54">
+        <v>51.40063</v>
+      </c>
+      <c r="C28" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="58" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="B10" s="39">
-        <v>40.793909999999997</v>
-      </c>
-      <c r="C10" s="41" t="s">
+      <c r="B29" s="54">
+        <v>54.493499999999997</v>
+      </c>
+      <c r="C29" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="D10" s="35" t="s">
-        <v>201</v>
-      </c>
-      <c r="E10" s="35"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="D29" s="58" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="B11" s="39">
-        <v>42.362909999999999</v>
-      </c>
-      <c r="C11" s="41" t="s">
+      <c r="B30" s="54">
+        <v>60.090139999999998</v>
+      </c>
+      <c r="C30" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="35" t="s">
-        <v>201</v>
-      </c>
-      <c r="E11" s="35"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="D30" s="58" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B31" s="54">
+        <v>15</v>
+      </c>
+      <c r="C31" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B32" s="54">
+        <v>3.6</v>
+      </c>
+      <c r="C32" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="E32" s="35" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="B33" s="54">
+        <v>5.65</v>
+      </c>
+      <c r="C33" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="E33" s="39"/>
+    </row>
+    <row r="34" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="B34" s="54">
+        <v>5.65</v>
+      </c>
+      <c r="C34" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="E34" s="39"/>
+    </row>
+    <row r="35" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B35" s="54">
+        <v>5.65</v>
+      </c>
+      <c r="C35" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="E35" s="39"/>
+    </row>
+    <row r="36" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B36" s="54">
+        <v>5.5</v>
+      </c>
+      <c r="C36" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="B12" s="39">
-        <v>24.47635</v>
-      </c>
-      <c r="C12" s="41" t="s">
+      <c r="E36" s="39"/>
+    </row>
+    <row r="37" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B37" s="54">
+        <v>5.5</v>
+      </c>
+      <c r="C37" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="D12" t="s">
-        <v>204</v>
-      </c>
-      <c r="E12" s="35"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
-        <v>149</v>
-      </c>
-      <c r="B13" s="39">
-        <v>15</v>
-      </c>
-      <c r="C13" s="41" t="s">
+      <c r="D37" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="E37" s="39"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B38" s="59">
+        <v>5.35</v>
+      </c>
+      <c r="C38" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="D13" t="s">
-        <v>226</v>
-      </c>
-      <c r="E13" s="35"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="35" t="s">
-        <v>131</v>
-      </c>
-      <c r="B14" s="39">
-        <v>5</v>
-      </c>
-      <c r="C14" s="41" t="s">
+      <c r="D38" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="E38" s="39"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="B39" s="59">
+        <v>5.35</v>
+      </c>
+      <c r="C39" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="D14" t="s">
-        <v>132</v>
-      </c>
-      <c r="E14" s="35"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
-        <v>164</v>
-      </c>
-      <c r="B15" s="39">
-        <v>5</v>
-      </c>
-      <c r="C15" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="35" t="s">
-        <v>132</v>
-      </c>
-      <c r="E15" s="35"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
-        <v>150</v>
-      </c>
-      <c r="B16" s="39">
-        <v>3.6</v>
-      </c>
-      <c r="C16" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D16" t="s">
-        <v>225</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="38" t="s">
-        <v>151</v>
-      </c>
-      <c r="B17" s="39">
-        <v>3.6</v>
-      </c>
-      <c r="C17" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="35" t="s">
-        <v>225</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="B18" s="39">
-        <v>2.7</v>
-      </c>
-      <c r="C18" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D18" t="s">
-        <v>226</v>
-      </c>
-      <c r="E18" s="35"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="38" t="s">
-        <v>165</v>
-      </c>
-      <c r="B19" s="39">
-        <v>0</v>
-      </c>
-      <c r="C19" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D19" t="s">
-        <v>163</v>
-      </c>
-      <c r="E19" s="35"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="B20" s="39">
-        <v>2.9</v>
-      </c>
-      <c r="C20" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D20" s="35" t="s">
-        <v>212</v>
-      </c>
-      <c r="E20" s="35"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
-        <v>207</v>
-      </c>
-      <c r="B21" s="39">
-        <v>2.9</v>
-      </c>
-      <c r="C21" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="35" t="s">
-        <v>212</v>
-      </c>
-      <c r="E21" s="35"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
-        <v>153</v>
-      </c>
-      <c r="B22" s="39">
-        <v>2.9</v>
-      </c>
-      <c r="C22" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" s="35" t="s">
-        <v>212</v>
-      </c>
-      <c r="E22" s="35"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
-        <v>154</v>
-      </c>
-      <c r="B23" s="39">
-        <v>2.746</v>
-      </c>
-      <c r="C23" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D23" s="35" t="s">
-        <v>213</v>
-      </c>
-      <c r="E23" s="35"/>
-    </row>
-    <row r="24" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35" t="s">
-        <v>208</v>
-      </c>
-      <c r="B24" s="39">
-        <v>2.746</v>
-      </c>
-      <c r="C24" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D24" s="35" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
-        <v>155</v>
-      </c>
-      <c r="B25" s="40">
-        <v>2.4321000000000002</v>
-      </c>
-      <c r="C25" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D25" s="35" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
-        <v>209</v>
-      </c>
-      <c r="B26" s="40">
-        <v>2.4321000000000002</v>
-      </c>
-      <c r="C26" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D26" s="35" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="35" t="s">
-        <v>210</v>
-      </c>
-      <c r="B27" s="40">
-        <v>2.4321000000000002</v>
-      </c>
-      <c r="C27" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D27" s="35" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="35" t="s">
-        <v>211</v>
-      </c>
-      <c r="B28" s="40">
-        <v>2.4321000000000002</v>
-      </c>
-      <c r="C28" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D28" s="35" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="B29" s="39">
-        <v>17.002960000000002</v>
-      </c>
-      <c r="C29" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D29" s="35" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
-        <v>220</v>
-      </c>
-      <c r="B30" s="39">
-        <v>17.002960000000002</v>
-      </c>
-      <c r="C30" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D30" s="35" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="B31" s="39">
-        <v>15.43505</v>
-      </c>
-      <c r="C31" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D31" s="35" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
-        <v>221</v>
-      </c>
-      <c r="B32" s="39">
-        <v>15.43505</v>
-      </c>
-      <c r="C32" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" s="35" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
-        <v>215</v>
-      </c>
-      <c r="B33" s="39">
-        <v>15.43505</v>
-      </c>
-      <c r="C33" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D33" s="35" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="35" t="s">
-        <v>216</v>
-      </c>
-      <c r="B34" s="39">
-        <v>15.43505</v>
-      </c>
-      <c r="C34" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D34" s="35" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="35" t="s">
-        <v>217</v>
-      </c>
-      <c r="B35" s="39">
-        <v>15.43505</v>
-      </c>
-      <c r="C35" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D35" s="35" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="35" t="s">
-        <v>218</v>
-      </c>
-      <c r="B36" s="39">
-        <v>15.43505</v>
-      </c>
-      <c r="C36" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D36" s="35" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="35" t="s">
-        <v>219</v>
-      </c>
-      <c r="B37" s="39">
-        <v>15.43505</v>
-      </c>
-      <c r="C37" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D37" s="35" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>135</v>
-      </c>
-      <c r="B38" s="39">
-        <v>20.064579999999999</v>
-      </c>
-      <c r="C38" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D38" s="35" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="B39" s="39">
-        <v>18.653790000000001</v>
-      </c>
-      <c r="C39" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D39" s="35" t="s">
-        <v>201</v>
-      </c>
+      <c r="D39" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="E39" s="39"/>
     </row>
     <row r="40" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="B40" s="39">
-        <v>15.048439999999999</v>
+        <v>206</v>
+      </c>
+      <c r="B40" s="40">
+        <v>5.35</v>
       </c>
       <c r="C40" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D40" s="35" t="s">
-        <v>201</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="E40" s="39"/>
     </row>
     <row r="41" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="35" t="s">
-        <v>124</v>
-      </c>
-      <c r="B41" s="39">
-        <v>83.306632489586676</v>
+        <v>207</v>
+      </c>
+      <c r="B41" s="40">
+        <v>5.35</v>
       </c>
       <c r="C41" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D41" s="35" t="s">
-        <v>201</v>
-      </c>
-      <c r="E41" s="35" t="s">
-        <v>174</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="E41" s="39"/>
     </row>
     <row r="42" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="35" t="s">
-        <v>125</v>
+        <v>166</v>
       </c>
       <c r="B42" s="39">
-        <v>51.806216746009525</v>
+        <v>3</v>
       </c>
       <c r="C42" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D42" s="35" t="s">
-        <v>201</v>
-      </c>
-      <c r="E42" s="35" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="35" t="s">
-        <v>126</v>
+        <v>160</v>
       </c>
       <c r="B43" s="39">
-        <v>32.875074716078899</v>
+        <v>8.7200000000000006</v>
       </c>
       <c r="C43" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D43" s="35" t="s">
-        <v>201</v>
-      </c>
-      <c r="E43" s="35" t="s">
-        <v>170</v>
+        <v>217</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="35" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="B44" s="39">
-        <v>195.56</v>
+        <v>8.64</v>
       </c>
       <c r="C44" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D44" s="35" t="s">
-        <v>201</v>
-      </c>
-      <c r="E44" s="35" t="s">
-        <v>171</v>
+        <v>217</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="35" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="B45" s="39">
-        <v>98.412999999999997</v>
+        <v>2.41</v>
       </c>
       <c r="C45" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D45" s="35" t="s">
-        <v>201</v>
-      </c>
-      <c r="E45" s="35" t="s">
-        <v>172</v>
+        <v>217</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="35" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B46" s="39">
-        <v>51.85</v>
+        <v>195.56</v>
       </c>
       <c r="C46" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="D46" s="35" t="s">
-        <v>201</v>
+      <c r="D46" s="53" t="s">
+        <v>237</v>
       </c>
       <c r="E46" s="35" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="35" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="B47" s="39">
-        <v>2.41</v>
+        <v>98.412999999999997</v>
       </c>
       <c r="C47" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="D47" s="35" t="s">
-        <v>226</v>
+      <c r="D47" s="53" t="s">
+        <v>237</v>
+      </c>
+      <c r="E47" s="35" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="35" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B48" s="39">
-        <v>8.64</v>
+        <v>51.85</v>
       </c>
       <c r="C48" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="D48" s="35" t="s">
-        <v>226</v>
-      </c>
-      <c r="E48" s="35"/>
+      <c r="D48" s="53" t="s">
+        <v>237</v>
+      </c>
+      <c r="E48" s="35" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="35" t="s">
-        <v>166</v>
-      </c>
-      <c r="B49" s="39">
-        <v>3</v>
+        <v>223</v>
+      </c>
+      <c r="B49" s="35">
+        <v>8</v>
       </c>
       <c r="C49" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D49" s="35" t="s">
-        <v>226</v>
-      </c>
-      <c r="E49" s="35"/>
+        <v>217</v>
+      </c>
+      <c r="E49" s="35" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="50" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="35" t="s">
-        <v>227</v>
-      </c>
-      <c r="B50" s="39">
-        <v>0</v>
+        <v>236</v>
+      </c>
+      <c r="B50" s="35">
+        <v>8</v>
       </c>
       <c r="C50" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D50" s="35" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="E50" s="35" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="35" t="s">
-        <v>160</v>
-      </c>
-      <c r="B51" s="39">
-        <v>8.7200000000000006</v>
+        <v>222</v>
+      </c>
+      <c r="B51" s="35">
+        <v>2.8</v>
       </c>
       <c r="C51" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D51" s="35" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="35" t="s">
-        <v>243</v>
+        <v>136</v>
       </c>
       <c r="B52" s="39">
-        <v>2.2999999999999998</v>
+        <v>13.03426</v>
       </c>
       <c r="C52" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="D52" s="35" t="s">
-        <v>226</v>
+      <c r="D52" s="53" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="35" t="s">
-        <v>158</v>
-      </c>
-      <c r="B53" s="39">
-        <v>8.64</v>
+        <v>137</v>
+      </c>
+      <c r="B53" s="52">
+        <v>12.886979999999999</v>
       </c>
       <c r="C53" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="D53" s="35" t="s">
-        <v>226</v>
+      <c r="D53" s="53" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="35" t="s">
-        <v>157</v>
-      </c>
-      <c r="B54" s="35">
-        <v>2.4</v>
+        <v>135</v>
+      </c>
+      <c r="B54" s="39">
+        <v>15.53801</v>
       </c>
       <c r="C54" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="D54" s="35" t="s">
-        <v>226</v>
+      <c r="D54" s="53" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -2877,214 +2967,218 @@
         <v>228</v>
       </c>
       <c r="B55" s="35">
-        <v>1.33</v>
+        <v>0</v>
       </c>
       <c r="C55" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D55" s="35" t="s">
-        <v>226</v>
+        <v>217</v>
+      </c>
+      <c r="E55" s="35" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="35" t="s">
-        <v>230</v>
+        <v>157</v>
       </c>
       <c r="B56" s="35">
-        <v>1</v>
+        <v>2.4</v>
       </c>
       <c r="C56" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D56" s="35" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="35" t="s">
-        <v>159</v>
+        <v>221</v>
       </c>
       <c r="B57" s="35">
-        <v>2.41</v>
+        <v>1</v>
       </c>
       <c r="C57" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D57" s="35" t="s">
-        <v>226</v>
-      </c>
-      <c r="E57" s="35" t="s">
-        <v>229</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="E57" s="35"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="35" t="s">
-        <v>161</v>
-      </c>
-      <c r="B58" s="35">
-        <v>8.84</v>
+        <v>218</v>
+      </c>
+      <c r="B58" s="39">
+        <v>0</v>
       </c>
       <c r="C58" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D58" s="35" t="s">
-        <v>226</v>
-      </c>
-      <c r="E58" s="35"/>
+        <v>217</v>
+      </c>
+      <c r="E58" s="35" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="35" t="s">
-        <v>231</v>
+        <v>161</v>
       </c>
       <c r="B59" s="35">
-        <v>2.8</v>
+        <v>8.84</v>
       </c>
       <c r="C59" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D59" s="35" t="s">
-        <v>226</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="E59" s="35"/>
     </row>
     <row r="60" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="35" t="s">
-        <v>246</v>
-      </c>
-      <c r="B60" s="35">
-        <v>8</v>
+        <v>233</v>
+      </c>
+      <c r="B60" s="39">
+        <v>2.2999999999999998</v>
       </c>
       <c r="C60" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D60" s="35" t="s">
-        <v>226</v>
-      </c>
-      <c r="E60" s="35" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="35" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="B61" s="35">
-        <v>8</v>
+        <v>1.33</v>
       </c>
       <c r="C61" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D61" s="35" t="s">
-        <v>226</v>
-      </c>
-      <c r="E61" s="35" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="35" t="s">
-        <v>235</v>
-      </c>
-      <c r="B62" s="35">
-        <v>8.8800000000000008</v>
+        <v>158</v>
+      </c>
+      <c r="B62" s="39">
+        <v>8.64</v>
       </c>
       <c r="C62" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D62" s="35" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="35" t="s">
-        <v>241</v>
+        <v>159</v>
       </c>
       <c r="B63" s="35">
-        <v>1.4</v>
+        <v>2.41</v>
       </c>
       <c r="C63" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D63" s="35" t="s">
-        <v>226</v>
+        <v>217</v>
+      </c>
+      <c r="E63" s="35" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="35" t="s">
-        <v>240</v>
+      <c r="A64" s="51" t="s">
+        <v>234</v>
       </c>
       <c r="B64" s="35">
-        <v>2.81</v>
+        <v>0</v>
       </c>
       <c r="C64" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D64" s="35" t="s">
-        <v>226</v>
+        <v>217</v>
+      </c>
+      <c r="E64" s="35" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="35" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="B65" s="35">
-        <v>9.375</v>
+        <v>8.8800000000000008</v>
       </c>
       <c r="C65" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D65" s="35" t="s">
-        <v>226</v>
-      </c>
-      <c r="E65" s="35" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="B66" s="35">
-        <v>8.68</v>
+        <v>124</v>
+      </c>
+      <c r="B66" s="39">
+        <v>83.306632489586676</v>
       </c>
       <c r="C66" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="D66" s="35" t="s">
-        <v>226</v>
+      <c r="D66" s="53" t="s">
+        <v>237</v>
+      </c>
+      <c r="E66" s="35" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="35" t="s">
-        <v>238</v>
-      </c>
-      <c r="B67" s="35">
-        <v>0</v>
+        <v>125</v>
+      </c>
+      <c r="B67" s="39">
+        <v>51.806216746009525</v>
       </c>
       <c r="C67" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="D67" s="35" t="s">
-        <v>226</v>
+      <c r="D67" s="53" t="s">
+        <v>237</v>
       </c>
       <c r="E67" s="35" t="s">
-        <v>239</v>
+        <v>169</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="51" t="s">
-        <v>244</v>
-      </c>
-      <c r="B68" s="35">
-        <v>0</v>
+      <c r="A68" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="B68" s="39">
+        <v>32.875074716078899</v>
       </c>
       <c r="C68" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="D68" s="35" t="s">
-        <v>226</v>
+      <c r="D68" s="53" t="s">
+        <v>237</v>
       </c>
       <c r="E68" s="35" t="s">
-        <v>239</v>
+        <v>170</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -3188,6 +3282,11 @@
       <c r="D87" s="35"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E1" xr:uid="{8BDDE9FA-34B5-487F-BD06-B5E05371CD58}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E68">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -19737,7 +19836,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20045,8 +20144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC3B418-F353-48F3-81CC-971E8DA13285}">
   <dimension ref="B1:C127"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A100" sqref="A1:B1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C1:C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20057,405 +20156,208 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C1" s="2" t="s">
-        <v>185</v>
-      </c>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="35"/>
-      <c r="C2" s="35" t="s">
-        <v>139</v>
-      </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="35"/>
-      <c r="C3" s="35" t="s">
-        <v>140</v>
-      </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="35"/>
-      <c r="C4" s="35" t="s">
-        <v>141</v>
-      </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="35"/>
-      <c r="C5" s="35" t="s">
-        <v>142</v>
-      </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="35"/>
-      <c r="C6" s="35" t="s">
-        <v>143</v>
-      </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="35"/>
-      <c r="C7" s="35" t="s">
-        <v>144</v>
-      </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="35"/>
-      <c r="C8" s="35" t="s">
-        <v>145</v>
-      </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="35"/>
-      <c r="C9" s="35" t="s">
-        <v>146</v>
-      </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="35"/>
-      <c r="C10" s="35" t="s">
-        <v>147</v>
-      </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="35"/>
-      <c r="C11" s="35" t="s">
-        <v>148</v>
-      </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="35"/>
-      <c r="C12" s="35" t="s">
-        <v>242</v>
-      </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="35"/>
-      <c r="C13" s="35" t="s">
-        <v>149</v>
-      </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="35"/>
-      <c r="C14" s="35" t="s">
-        <v>131</v>
-      </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="35"/>
-      <c r="C15" s="35" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="35"/>
-      <c r="C16" s="35" t="s">
-        <v>150</v>
-      </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="35"/>
-      <c r="C17" s="38" t="s">
-        <v>151</v>
-      </c>
+      <c r="C17" s="38"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="35"/>
-      <c r="C18" s="38" t="s">
-        <v>152</v>
-      </c>
+      <c r="C18" s="38"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="35"/>
-      <c r="C19" s="38" t="s">
-        <v>165</v>
-      </c>
+      <c r="C19" s="38"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="35"/>
-      <c r="C20" s="35" t="s">
-        <v>206</v>
-      </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="35"/>
-      <c r="C21" s="35" t="s">
-        <v>207</v>
-      </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="35"/>
-      <c r="C22" s="35" t="s">
-        <v>153</v>
-      </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="35"/>
-      <c r="C23" s="35" t="s">
-        <v>154</v>
-      </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="35"/>
-      <c r="C24" s="35" t="s">
-        <v>208</v>
-      </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="35"/>
-      <c r="C25" s="35" t="s">
-        <v>155</v>
-      </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="35"/>
-      <c r="C26" s="35" t="s">
-        <v>209</v>
-      </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="35"/>
-      <c r="C27" s="35" t="s">
-        <v>210</v>
-      </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="35"/>
-      <c r="C28" s="35" t="s">
-        <v>211</v>
-      </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="35"/>
-      <c r="C29" s="35" t="s">
-        <v>133</v>
-      </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="35"/>
-      <c r="C30" s="35" t="s">
-        <v>220</v>
-      </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="35"/>
-      <c r="C31" s="35" t="s">
-        <v>134</v>
-      </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="35"/>
-      <c r="C32" s="35" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="35"/>
-      <c r="C33" s="35" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="35"/>
-      <c r="C34" s="35" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="35"/>
-      <c r="C35" s="35" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="35"/>
-      <c r="C36" s="35" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="35"/>
-      <c r="C37" s="35" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="35"/>
-      <c r="C38" s="35" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="35"/>
-      <c r="C39" s="35" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="35"/>
-      <c r="C40" s="35" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="35"/>
-      <c r="C41" s="35" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="35"/>
-      <c r="C42" s="35" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="35"/>
-      <c r="C43" s="35" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="35"/>
-      <c r="C44" s="35" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="35"/>
-      <c r="C45" s="35" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="35"/>
-      <c r="C46" s="35" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="35"/>
-      <c r="C47" s="35" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="35"/>
-      <c r="C48" s="35" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="35"/>
-      <c r="C49" s="35" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="35"/>
-      <c r="C50" s="35" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="35"/>
-      <c r="C51" s="35" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="35"/>
-      <c r="C52" s="35" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" s="35"/>
-      <c r="C53" s="35" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="35"/>
-      <c r="C54" s="35" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="35"/>
-      <c r="C55" s="35" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="35"/>
-      <c r="C56" s="35" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="35"/>
-      <c r="C57" s="35" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" s="35"/>
-      <c r="C58" s="35" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="35"/>
-      <c r="C59" s="35" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="35"/>
-      <c r="C60" s="35" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="35"/>
-      <c r="C61" s="35" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" s="35"/>
-      <c r="C62" s="35" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" s="35"/>
-      <c r="C63" s="35" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" s="35"/>
-      <c r="C64" s="35" t="s">
-        <v>240</v>
-      </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="35"/>
-      <c r="C65" s="35" t="s">
-        <v>236</v>
-      </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="35"/>
-      <c r="C66" s="35" t="s">
-        <v>237</v>
-      </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="35"/>
-      <c r="C67" s="35" t="s">
-        <v>238</v>
-      </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="35"/>

</xml_diff>